<commit_message>
Statutory Report Code changes
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeMonthly201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeMonthly201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Scottish Payroll InputSheet creations\Scottish Input sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="210" windowWidth="14340" windowHeight="4335" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="4335" windowWidth="14340" xWindow="390" yWindow="210"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="GeneralTaxRateMonthly" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForMonthlyTax" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="GeneralTaxRateMonthly" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForMonthlyTax" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="70">
   <si>
     <t>TC</t>
   </si>
@@ -238,6 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,69 +325,69 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -403,10 +404,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -441,7 +442,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,7 +494,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -598,7 +599,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -607,13 +608,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -623,7 +624,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -632,7 +633,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -641,7 +642,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -651,12 +652,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -687,7 +688,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -706,7 +707,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -718,7 +719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -727,10 +728,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="35.450000000000003" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -761,7 +762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -804,13 +805,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
@@ -819,17 +820,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -855,7 +856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>63</v>
       </c>
@@ -875,7 +876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.6" r="3" s="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>35</v>
       </c>
@@ -895,7 +896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
@@ -915,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -935,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
@@ -955,7 +956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
@@ -975,7 +976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -995,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>42</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>44</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>45</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>53</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
@@ -1175,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>55</v>
       </c>
@@ -1195,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>56</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="20" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -1237,15 +1238,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ" r:id="rId1" ref="A3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -1254,20 +1255,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="51.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="113.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="51.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="113.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="2" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="3" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>34</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="4" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="5" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="6" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="7" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="8" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="9" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="10" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="11" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="12" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="13" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -1728,7 +1729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="14" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1763,7 +1764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="15" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="16" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>34</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="17" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="18" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="19" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="20" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>34</v>
       </c>
@@ -1975,16 +1976,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2:A13" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ"/>
-    <hyperlink ref="A14:A20" r:id="rId3" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2:A13"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ" r:id="rId2" ref="B3"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId3" ref="A14:A20"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1993,21 +1994,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="52.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="67.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="52.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="67.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -2091,9 +2092,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
uploaded corrupt scottish input files
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeMonthly201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeMonthly201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Scottish Payroll InputSheet creations\Scottish Input sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="4335" windowWidth="14340" xWindow="390" yWindow="210"/>
+    <workbookView xWindow="390" yWindow="210" windowWidth="14340" windowHeight="4335" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="GeneralTaxRateMonthly" r:id="rId2" sheetId="2"/>
-    <sheet name="ProcessPayrollForMonthlyTax" r:id="rId3" sheetId="4"/>
-    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="GeneralTaxRateMonthly" sheetId="2" r:id="rId2"/>
+    <sheet name="ProcessPayrollForMonthlyTax" sheetId="4" r:id="rId3"/>
+    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="70">
   <si>
     <t>TC</t>
   </si>
@@ -238,7 +238,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,69 +324,69 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="2">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -404,10 +403,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -442,7 +441,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -599,7 +598,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -608,13 +607,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -624,7 +623,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -633,7 +632,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -642,7 +641,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -652,12 +651,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -688,7 +687,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -707,7 +706,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -719,7 +718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -728,10 +727,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -748,7 +747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="35.450000000000003" r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -762,7 +761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="30" r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -805,13 +804,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
@@ -820,17 +819,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -856,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>63</v>
       </c>
@@ -876,7 +875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="21.6" r="3" s="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>35</v>
       </c>
@@ -896,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
@@ -916,7 +915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -936,7 +935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
@@ -956,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
@@ -976,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="8" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -996,7 +995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="9" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
@@ -1016,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="10" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>42</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -1056,7 +1055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>44</v>
       </c>
@@ -1076,7 +1075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>45</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="14" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
@@ -1116,7 +1115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="15" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>53</v>
       </c>
@@ -1156,7 +1155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
@@ -1176,7 +1175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>55</v>
       </c>
@@ -1196,7 +1195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>56</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="20" s="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -1238,15 +1237,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ" r:id="rId1" ref="A3"/>
+    <hyperlink ref="A3" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -1255,20 +1254,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="51.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="113.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="113.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="2" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="3" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>34</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="4" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1414,7 +1413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="5" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="6" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="7" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="8" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="9" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1589,7 +1588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="10" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="11" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="12" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="13" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="14" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1764,7 +1763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="15" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="16" s="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>34</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="17" s="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="18" s="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="19" s="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="20" s="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>34</v>
       </c>
@@ -1976,16 +1975,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2:A13"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ" r:id="rId2" ref="B3"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId3" ref="A14:A20"/>
+    <hyperlink ref="A2:A13" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ"/>
+    <hyperlink ref="A14:A20" r:id="rId3" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1994,21 +1993,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="52.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="67.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="67.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.9" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -2092,9 +2091,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scottish Module Input files modification
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeMonthly201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeMonthly201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Scottish Payroll InputSheet creations\Scottish Input sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="210" windowWidth="14340" windowHeight="4335" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="4335" windowWidth="14340" xWindow="390" yWindow="210"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="GeneralTaxRateMonthly" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForMonthlyTax" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="GeneralTaxRateMonthly" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForMonthlyTax" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="70">
   <si>
     <t>TC</t>
   </si>
@@ -238,6 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,69 +325,69 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -403,10 +404,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -441,7 +442,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,7 +494,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -598,7 +599,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -607,13 +608,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -623,7 +624,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -632,7 +633,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -641,7 +642,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -651,12 +652,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -687,7 +688,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -706,7 +707,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -718,7 +719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -727,10 +728,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="35.450000000000003" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -761,7 +762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -804,13 +805,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
@@ -819,17 +820,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -855,7 +856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>63</v>
       </c>
@@ -875,7 +876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.6" r="3" s="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>35</v>
       </c>
@@ -895,7 +896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
@@ -915,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -935,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
@@ -955,7 +956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
@@ -975,7 +976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -995,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>42</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>44</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>45</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>53</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
@@ -1175,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>55</v>
       </c>
@@ -1195,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>56</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="20" s="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -1237,15 +1238,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ" r:id="rId1" ref="A3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -1254,20 +1255,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="51.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="113.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="51.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="113.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="2" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="3" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>34</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="4" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="5" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="6" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="7" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="8" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="9" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="10" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="11" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="12" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="13" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -1728,7 +1729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="14" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1763,7 +1764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="15" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="16" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>34</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="17" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="18" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="19" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="20" s="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>34</v>
       </c>
@@ -1975,16 +1976,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2:A13" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ"/>
-    <hyperlink ref="A14:A20" r:id="rId3" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2:A13"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Tb000000eqWAJ" r:id="rId2" ref="B3"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId3" ref="A14:A20"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1993,21 +1994,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="52.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="67.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="52.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="67.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.9" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -2091,9 +2092,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>